<commit_message>
fix hmsartnr missing 0
</commit_message>
<xml_diff>
--- a/src/main/resources/substituttlister/V10_vogner.xlsx
+++ b/src/main/resources/substituttlister/V10_vogner.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasmund/dev/hm-grunndata-alternativprodukter/src/main/resources/substituttlister/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinhanhtuantran/dev/navikt/hm/hm-grunndata-alternativprodukter/src/main/resources/substituttlister/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF96101-6CB3-CB41-B6A0-65AF6F7BF675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77902454-1668-0643-AA34-A0206888CD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16560" firstSheet="1" activeTab="1" xr2:uid="{DAB7D3D8-04D0-4DD5-9B74-78B882D95CED}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="349">
   <si>
     <t>Delkontrakt</t>
   </si>
@@ -1077,6 +1077,15 @@
   </si>
   <si>
     <t>123458</t>
+  </si>
+  <si>
+    <t>190454</t>
+  </si>
+  <si>
+    <t>072427</t>
+  </si>
+  <si>
+    <t>038639</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1244,25 +1253,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2575,8 +2581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3485A8-7267-48FD-BE99-693AE922852B}">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2604,7 +2610,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="32"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2620,7 +2626,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="G2" s="32"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -2632,7 +2638,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="G3" s="32"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -2644,7 +2650,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="G4" s="32"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
@@ -2656,7 +2662,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="G5" s="32"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -2668,7 +2674,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="G6" s="32"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -2680,7 +2686,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="G7" s="32"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -2692,7 +2698,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="G8" s="32"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -2704,7 +2710,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="G9" s="32"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -2716,7 +2722,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="G10" s="32"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -2728,13 +2734,13 @@
         <v>25</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="G11" s="32"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="G12" s="32"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -2750,7 +2756,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="G13" s="32"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -2762,13 +2768,13 @@
         <v>31</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="G14" s="32"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="G15" s="32"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -2784,7 +2790,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="G16" s="32"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
@@ -2795,7 +2801,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="G17" s="32"/>
+      <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
@@ -2806,7 +2812,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="G18" s="32"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
@@ -2817,7 +2823,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="G19" s="32"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
@@ -2828,7 +2834,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="G20" s="32"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
@@ -2839,7 +2845,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="G21" s="32"/>
+      <c r="G21" s="28"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
@@ -2850,7 +2856,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="G22" s="32"/>
+      <c r="G22" s="28"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
@@ -2861,7 +2867,7 @@
         <v>49</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="G23" s="32"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
@@ -2872,26 +2878,26 @@
         <v>51</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="G24" s="32"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="32"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="28"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="G26" s="32"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -2907,7 +2913,7 @@
         <v>58</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="G27" s="32"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
@@ -2918,7 +2924,7 @@
         <v>60</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="G28" s="32"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
@@ -2929,12 +2935,12 @@
         <v>62</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="G29" s="32"/>
+      <c r="G29" s="28"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="G30" s="32"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -2950,7 +2956,7 @@
         <v>66</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="G31" s="32"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
@@ -2963,7 +2969,7 @@
       <c r="E32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G32" s="32"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
@@ -2976,7 +2982,7 @@
       <c r="E33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G33" s="32"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
@@ -2987,7 +2993,7 @@
         <v>73</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="G34" s="32"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
@@ -2998,7 +3004,7 @@
         <v>75</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="G35" s="32"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
@@ -3009,7 +3015,7 @@
         <v>77</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="G36" s="32"/>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
@@ -3022,12 +3028,12 @@
       <c r="E37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G37" s="32"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="G38" s="32"/>
+      <c r="G38" s="28"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
@@ -3043,7 +3049,7 @@
         <v>83</v>
       </c>
       <c r="E39" s="1"/>
-      <c r="G39" s="32"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
@@ -3054,7 +3060,7 @@
         <v>85</v>
       </c>
       <c r="E40" s="1"/>
-      <c r="G40" s="32"/>
+      <c r="G40" s="28"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
@@ -3065,7 +3071,7 @@
         <v>87</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="G41" s="32"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
@@ -3076,7 +3082,7 @@
         <v>89</v>
       </c>
       <c r="E42" s="1"/>
-      <c r="G42" s="32"/>
+      <c r="G42" s="28"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
@@ -3087,7 +3093,7 @@
         <v>91</v>
       </c>
       <c r="E43" s="1"/>
-      <c r="G43" s="32"/>
+      <c r="G43" s="28"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
@@ -3098,7 +3104,7 @@
         <v>93</v>
       </c>
       <c r="E44" s="1"/>
-      <c r="G44" s="32"/>
+      <c r="G44" s="28"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
@@ -3109,25 +3115,25 @@
         <v>95</v>
       </c>
       <c r="E45" s="1"/>
-      <c r="G45" s="32"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
-      <c r="C46" s="30" t="s">
+      <c r="C46" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="G46" s="32"/>
+      <c r="G46" s="28"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="G47" s="32"/>
+      <c r="G47" s="28"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
@@ -3143,7 +3149,7 @@
         <v>102</v>
       </c>
       <c r="E48" s="1"/>
-      <c r="G48" s="32"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
@@ -3154,7 +3160,7 @@
         <v>104</v>
       </c>
       <c r="E49" s="1"/>
-      <c r="G49" s="32"/>
+      <c r="G49" s="28"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
@@ -3165,7 +3171,7 @@
         <v>106</v>
       </c>
       <c r="E50" s="1"/>
-      <c r="G50" s="32"/>
+      <c r="G50" s="28"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
@@ -3176,7 +3182,7 @@
         <v>108</v>
       </c>
       <c r="E51" s="1"/>
-      <c r="G51" s="32"/>
+      <c r="G51" s="28"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
@@ -3186,7 +3192,7 @@
         <v>110</v>
       </c>
       <c r="E52" s="1"/>
-      <c r="G52" s="32"/>
+      <c r="G52" s="28"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
@@ -3197,7 +3203,7 @@
         <v>106</v>
       </c>
       <c r="E53" s="1"/>
-      <c r="G53" s="32"/>
+      <c r="G53" s="28"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
@@ -3208,7 +3214,7 @@
         <v>112</v>
       </c>
       <c r="E54" s="1"/>
-      <c r="G54" s="32"/>
+      <c r="G54" s="28"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
@@ -3219,7 +3225,7 @@
         <v>114</v>
       </c>
       <c r="E55" s="1"/>
-      <c r="G55" s="32"/>
+      <c r="G55" s="28"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
@@ -3230,7 +3236,7 @@
         <v>116</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="G56" s="32"/>
+      <c r="G56" s="28"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
@@ -3241,7 +3247,7 @@
         <v>118</v>
       </c>
       <c r="E57" s="1"/>
-      <c r="G57" s="32"/>
+      <c r="G57" s="28"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
@@ -3252,18 +3258,18 @@
         <v>120</v>
       </c>
       <c r="E58" s="1"/>
-      <c r="G58" s="32"/>
+      <c r="G58" s="28"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
-      <c r="C59" s="30" t="s">
+      <c r="C59" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="26" t="s">
         <v>122</v>
       </c>
       <c r="E59" s="1"/>
-      <c r="G59" s="32"/>
+      <c r="G59" s="28"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
@@ -3274,12 +3280,12 @@
         <v>124</v>
       </c>
       <c r="E60" s="1"/>
-      <c r="G60" s="32"/>
+      <c r="G60" s="28"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="G61" s="32"/>
+      <c r="G61" s="28"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
@@ -3291,33 +3297,33 @@
       <c r="C62" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="25" t="s">
         <v>128</v>
       </c>
       <c r="E62" s="1"/>
-      <c r="G62" s="32"/>
+      <c r="G62" s="28"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B63" s="21"/>
       <c r="C63" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D63" s="25" t="s">
         <v>130</v>
       </c>
       <c r="E63" s="1"/>
-      <c r="G63" s="32"/>
+      <c r="G63" s="28"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B64" s="21"/>
       <c r="C64" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="D64" s="28" t="s">
+      <c r="D64" s="25" t="s">
         <v>132</v>
       </c>
       <c r="E64" s="1"/>
-      <c r="G64" s="32"/>
+      <c r="G64" s="28"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B65" s="21"/>
@@ -3328,43 +3334,42 @@
         <v>134</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="G65" s="32"/>
+      <c r="G65" s="28"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
         <v>135</v>
       </c>
-      <c r="D66" s="23">
+      <c r="D66" s="22">
         <v>286305</v>
       </c>
       <c r="E66" s="1"/>
-      <c r="G66" s="32"/>
+      <c r="G66" s="28"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
         <v>136</v>
       </c>
-      <c r="D67" s="23">
+      <c r="D67" s="22">
         <v>286306</v>
       </c>
       <c r="E67" s="1"/>
-      <c r="G67" s="32"/>
+      <c r="G67" s="28"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
         <v>137</v>
       </c>
-      <c r="D68" s="23">
+      <c r="D68" s="22">
         <v>286307</v>
       </c>
       <c r="E68" s="1"/>
-      <c r="G68" s="32"/>
+      <c r="G68" s="28"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C69"/>
-      <c r="D69"/>
       <c r="E69" s="1"/>
-      <c r="G69" s="32"/>
+      <c r="G69" s="28"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
@@ -3376,127 +3381,127 @@
       <c r="C70" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="D70" s="24">
+      <c r="D70" s="25">
         <v>325280</v>
       </c>
       <c r="E70" s="1"/>
-      <c r="G70" s="32"/>
+      <c r="G70" s="28"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C71" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="D71" s="24">
+      <c r="D71" s="25">
         <v>325281</v>
       </c>
       <c r="E71" s="1"/>
-      <c r="G71" s="32"/>
+      <c r="G71" s="28"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C72" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="D72" s="24">
+      <c r="D72" s="25">
         <v>325282</v>
       </c>
       <c r="E72" s="1"/>
-      <c r="G72" s="32"/>
+      <c r="G72" s="28"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C73" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="D73" s="24">
+      <c r="D73" s="25">
         <v>324998</v>
       </c>
       <c r="E73" s="1"/>
-      <c r="G73" s="32"/>
+      <c r="G73" s="28"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C74" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="D74" s="24">
+      <c r="D74" s="25">
         <v>324999</v>
       </c>
       <c r="E74" s="1"/>
-      <c r="G74" s="32"/>
+      <c r="G74" s="28"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>145</v>
       </c>
-      <c r="D75" s="23">
+      <c r="D75" s="22">
         <v>285561</v>
       </c>
       <c r="E75" s="1"/>
-      <c r="G75" s="32"/>
+      <c r="G75" s="28"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
         <v>146</v>
       </c>
-      <c r="D76" s="23">
+      <c r="D76" s="22">
         <v>231718</v>
       </c>
-      <c r="G76" s="32"/>
+      <c r="G76" s="28"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="25">
+      <c r="D77" s="29">
         <v>285784</v>
       </c>
-      <c r="G77" s="32"/>
+      <c r="G77" s="28"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
         <v>148</v>
       </c>
-      <c r="D78" s="23">
+      <c r="D78" s="22">
         <v>285785</v>
       </c>
-      <c r="G78" s="32"/>
+      <c r="G78" s="28"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
         <v>149</v>
       </c>
-      <c r="D79" s="25">
+      <c r="D79" s="29">
         <v>311301</v>
       </c>
-      <c r="G79" s="32"/>
+      <c r="G79" s="28"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
         <v>150</v>
       </c>
-      <c r="D80" s="23">
+      <c r="D80" s="22">
         <v>313141</v>
       </c>
-      <c r="G80" s="32"/>
+      <c r="G80" s="28"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
         <v>151</v>
       </c>
-      <c r="D81" s="25">
+      <c r="D81" s="29">
         <v>322218</v>
       </c>
-      <c r="G81" s="32"/>
+      <c r="G81" s="28"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
         <v>152</v>
       </c>
-      <c r="D82" s="25">
+      <c r="D82" s="29">
         <v>298488</v>
       </c>
-      <c r="G82" s="32"/>
+      <c r="G82" s="28"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G83" s="32"/>
+      <c r="G83" s="28"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
@@ -3508,94 +3513,94 @@
       <c r="C84" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D84" s="24">
+      <c r="D84" s="25">
         <v>324592</v>
       </c>
-      <c r="G84" s="32"/>
+      <c r="G84" s="28"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C85" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="D85" s="24">
+      <c r="D85" s="25">
         <v>324593</v>
       </c>
-      <c r="G85" s="32"/>
+      <c r="G85" s="28"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C86" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="D86" s="24">
+      <c r="D86" s="25">
         <v>324996</v>
       </c>
-      <c r="G86" s="32"/>
+      <c r="G86" s="28"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C87" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="D87" s="24">
+      <c r="D87" s="25">
         <v>324997</v>
       </c>
-      <c r="G87" s="32"/>
+      <c r="G87" s="28"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
         <v>159</v>
       </c>
-      <c r="D88" s="23">
+      <c r="D88" s="22">
         <v>232525</v>
       </c>
-      <c r="G88" s="32"/>
+      <c r="G88" s="28"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="23">
+      <c r="D89" s="22">
         <v>232526</v>
       </c>
-      <c r="G89" s="32"/>
+      <c r="G89" s="28"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
         <v>161</v>
       </c>
-      <c r="D90" s="23">
+      <c r="D90" s="22">
         <v>285562</v>
       </c>
-      <c r="G90" s="32"/>
+      <c r="G90" s="28"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
         <v>162</v>
       </c>
-      <c r="D91" s="23">
+      <c r="D91" s="22">
         <v>231921</v>
       </c>
-      <c r="G91" s="32"/>
+      <c r="G91" s="28"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
         <v>163</v>
       </c>
-      <c r="D92" s="23">
+      <c r="D92" s="22">
         <v>234364</v>
       </c>
-      <c r="G92" s="32"/>
+      <c r="G92" s="28"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C93" s="26" t="s">
+      <c r="C93" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="D93" s="27">
-        <v>190454</v>
-      </c>
-      <c r="G93" s="32"/>
+      <c r="D93" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="G93" s="28"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G94" s="32"/>
+      <c r="G94" s="28"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
@@ -3607,166 +3612,166 @@
       <c r="C95" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="D95" s="24">
+      <c r="D95" s="25">
         <v>324995</v>
       </c>
-      <c r="G95" s="32"/>
+      <c r="G95" s="28"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C96" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="D96" s="24">
+      <c r="D96" s="25">
         <v>324879</v>
       </c>
-      <c r="G96" s="32"/>
+      <c r="G96" s="28"/>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C97" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="D97" s="24">
+      <c r="D97" s="25">
         <v>324880</v>
       </c>
-      <c r="G97" s="32"/>
+      <c r="G97" s="28"/>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C98" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="D98" s="24">
+      <c r="D98" s="25">
         <v>269654</v>
       </c>
-      <c r="G98" s="32"/>
+      <c r="G98" s="28"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C99" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="D99" s="24">
+      <c r="D99" s="25">
         <v>269829</v>
       </c>
-      <c r="G99" s="32"/>
+      <c r="G99" s="28"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C100" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="D100" s="24">
+      <c r="D100" s="25">
         <v>269920</v>
       </c>
-      <c r="G100" s="32"/>
+      <c r="G100" s="28"/>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C101" s="26" t="s">
+      <c r="C101" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="D101" s="27">
-        <v>72427</v>
-      </c>
-      <c r="G101" s="32"/>
+      <c r="D101" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G101" s="28"/>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
         <v>174</v>
       </c>
-      <c r="D102" s="23">
+      <c r="D102" s="22">
         <v>146011</v>
       </c>
-      <c r="G102" s="32"/>
+      <c r="G102" s="28"/>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
         <v>175</v>
       </c>
-      <c r="D103" s="23">
+      <c r="D103" s="22">
         <v>231864</v>
       </c>
-      <c r="G103" s="32"/>
+      <c r="G103" s="28"/>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
         <v>176</v>
       </c>
-      <c r="D104" s="23">
+      <c r="D104" s="22">
         <v>231863</v>
       </c>
-      <c r="G104" s="32"/>
+      <c r="G104" s="28"/>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
         <v>177</v>
       </c>
-      <c r="D105" s="23">
+      <c r="D105" s="22">
         <v>231862</v>
       </c>
-      <c r="G105" s="32"/>
+      <c r="G105" s="28"/>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C106" t="s">
         <v>178</v>
       </c>
-      <c r="D106" s="23">
+      <c r="D106" s="22">
         <v>231861</v>
       </c>
-      <c r="G106" s="32"/>
+      <c r="G106" s="28"/>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
         <v>179</v>
       </c>
-      <c r="D107" s="23">
+      <c r="D107" s="22">
         <v>231860</v>
       </c>
-      <c r="G107" s="32"/>
+      <c r="G107" s="28"/>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C108" t="s">
         <v>180</v>
       </c>
-      <c r="D108" s="23">
+      <c r="D108" s="22">
         <v>231859</v>
       </c>
-      <c r="G108" s="32"/>
+      <c r="G108" s="28"/>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C109" t="s">
         <v>181</v>
       </c>
-      <c r="D109" s="23">
+      <c r="D109" s="22">
         <v>232330</v>
       </c>
-      <c r="G109" s="32"/>
+      <c r="G109" s="28"/>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C110" t="s">
         <v>182</v>
       </c>
-      <c r="D110" s="23">
+      <c r="D110" s="22">
         <v>230300</v>
       </c>
-      <c r="G110" s="32"/>
+      <c r="G110" s="28"/>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C111" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="D111" s="23">
+      <c r="D111" s="22">
         <v>232331</v>
       </c>
-      <c r="G111" s="32"/>
+      <c r="G111" s="28"/>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C112" s="26" t="s">
+      <c r="C112" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="D112" s="27">
+      <c r="D112" s="30">
         <v>190453</v>
       </c>
-      <c r="G112" s="32"/>
+      <c r="G112" s="28"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G113" s="32"/>
+      <c r="G113" s="28"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
@@ -3778,157 +3783,157 @@
       <c r="C114" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="D114" s="24">
+      <c r="D114" s="25">
         <v>313168</v>
       </c>
-      <c r="G114" s="32"/>
+      <c r="G114" s="28"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C115" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="D115" s="24">
+      <c r="D115" s="25">
         <v>312498</v>
       </c>
-      <c r="G115" s="32"/>
+      <c r="G115" s="28"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C116" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="D116" s="24">
+      <c r="D116" s="25">
         <v>312687</v>
       </c>
-      <c r="G116" s="32"/>
+      <c r="G116" s="28"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C117" t="s">
         <v>190</v>
       </c>
-      <c r="D117" s="23">
+      <c r="D117" s="22">
         <v>296508</v>
       </c>
-      <c r="G117" s="32"/>
+      <c r="G117" s="28"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C118" t="s">
         <v>191</v>
       </c>
-      <c r="D118" s="23">
+      <c r="D118" s="22">
         <v>296509</v>
       </c>
-      <c r="G118" s="32"/>
+      <c r="G118" s="28"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C119" t="s">
         <v>192</v>
       </c>
-      <c r="D119" s="23">
+      <c r="D119" s="22">
         <v>296510</v>
       </c>
-      <c r="G119" s="32"/>
+      <c r="G119" s="28"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C120" t="s">
         <v>193</v>
       </c>
-      <c r="D120" s="23">
+      <c r="D120" s="22">
         <v>292379</v>
       </c>
-      <c r="G120" s="32"/>
+      <c r="G120" s="28"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C121" s="26" t="s">
+      <c r="C121" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="D121" s="27">
+      <c r="D121" s="30">
         <v>144161</v>
       </c>
-      <c r="G121" s="32"/>
+      <c r="G121" s="28"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C122" s="26" t="s">
+      <c r="C122" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="D122" s="27">
+      <c r="D122" s="30">
         <v>269907</v>
       </c>
-      <c r="G122" s="32"/>
+      <c r="G122" s="28"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C123" s="26" t="s">
+      <c r="C123" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="D123" s="27">
+      <c r="D123" s="30">
         <v>253316</v>
       </c>
-      <c r="G123" s="32"/>
+      <c r="G123" s="28"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C124" s="26" t="s">
+      <c r="C124" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="D124" s="27">
+      <c r="D124" s="30">
         <v>253346</v>
       </c>
-      <c r="G124" s="32"/>
+      <c r="G124" s="28"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C125" s="26" t="s">
+      <c r="C125" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="D125" s="27">
+      <c r="D125" s="30">
         <v>253341</v>
       </c>
-      <c r="G125" s="32"/>
+      <c r="G125" s="28"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C126" s="26" t="s">
+      <c r="C126" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="D126" s="27">
+      <c r="D126" s="30">
         <v>270150</v>
       </c>
-      <c r="G126" s="32"/>
+      <c r="G126" s="28"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C127" s="26" t="s">
+      <c r="C127" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="D127" s="27">
+      <c r="D127" s="30">
         <v>253372</v>
       </c>
-      <c r="G127" s="32"/>
+      <c r="G127" s="28"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C128" t="s">
         <v>201</v>
       </c>
-      <c r="D128" s="23">
+      <c r="D128" s="22">
         <v>318370</v>
       </c>
-      <c r="G128" s="32"/>
+      <c r="G128" s="28"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C129" t="s">
         <v>202</v>
       </c>
-      <c r="D129" s="29">
+      <c r="D129" s="31">
         <v>313819</v>
       </c>
-      <c r="G129" s="32"/>
+      <c r="G129" s="28"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C130" t="s">
         <v>203</v>
       </c>
-      <c r="D130" s="23">
+      <c r="D130" s="22">
         <v>327971</v>
       </c>
-      <c r="G130" s="32"/>
+      <c r="G130" s="28"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G131" s="32"/>
+      <c r="G131" s="28"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
@@ -3940,50 +3945,50 @@
       <c r="C132" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="D132" s="24">
+      <c r="D132" s="25">
         <v>324745</v>
       </c>
-      <c r="G132" s="32"/>
+      <c r="G132" s="28"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C133" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="D133" s="24">
+      <c r="D133" s="25">
         <v>324746</v>
       </c>
-      <c r="G133" s="32"/>
+      <c r="G133" s="28"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C134" t="s">
         <v>208</v>
       </c>
-      <c r="D134" s="23">
+      <c r="D134" s="22">
         <v>164300</v>
       </c>
-      <c r="G134" s="32"/>
+      <c r="G134" s="28"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C135" t="s">
         <v>209</v>
       </c>
-      <c r="D135" s="23">
+      <c r="D135" s="22">
         <v>215285</v>
       </c>
-      <c r="G135" s="32"/>
+      <c r="G135" s="28"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C136" t="s">
         <v>210</v>
       </c>
-      <c r="D136" s="23">
+      <c r="D136" s="22">
         <v>287188</v>
       </c>
-      <c r="G136" s="32"/>
+      <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D137" s="22"/>
-      <c r="G137" s="32"/>
+      <c r="G137" s="28"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
@@ -3995,40 +4000,40 @@
       <c r="C138" t="s">
         <v>213</v>
       </c>
-      <c r="D138" s="23">
+      <c r="D138" s="22">
         <v>230015</v>
       </c>
-      <c r="G138" s="32"/>
+      <c r="G138" s="28"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C139" t="s">
         <v>214</v>
       </c>
-      <c r="D139" s="23">
+      <c r="D139" s="22">
         <v>230196</v>
       </c>
-      <c r="G139" s="32"/>
+      <c r="G139" s="28"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C140" t="s">
         <v>215</v>
       </c>
-      <c r="D140" s="23">
+      <c r="D140" s="22">
         <v>286265</v>
       </c>
-      <c r="G140" s="32"/>
+      <c r="G140" s="28"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C141" t="s">
         <v>216</v>
       </c>
-      <c r="D141" s="23">
+      <c r="D141" s="22">
         <v>327024</v>
       </c>
-      <c r="G141" s="32"/>
+      <c r="G141" s="28"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G142" s="32"/>
+      <c r="G142" s="28"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
@@ -4040,58 +4045,58 @@
       <c r="C143" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D143" s="24">
+      <c r="D143" s="25">
         <v>285563</v>
       </c>
-      <c r="G143" s="32"/>
+      <c r="G143" s="28"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C144" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D144" s="24">
+      <c r="D144" s="25">
         <v>285564</v>
       </c>
-      <c r="G144" s="32"/>
+      <c r="G144" s="28"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C145" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D145" s="24">
+      <c r="D145" s="25">
         <v>285565</v>
       </c>
-      <c r="G145" s="32"/>
+      <c r="G145" s="28"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C146" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D146" s="24">
+      <c r="D146" s="25">
         <v>285566</v>
       </c>
-      <c r="G146" s="32"/>
+      <c r="G146" s="28"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C147" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D147" s="27">
-        <v>38639</v>
-      </c>
-      <c r="G147" s="32"/>
+      <c r="D147" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="G147" s="28"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C148" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D148" s="27">
+      <c r="D148" s="30">
         <v>147233</v>
       </c>
-      <c r="G148" s="32"/>
+      <c r="G148" s="28"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G149" s="32"/>
+      <c r="G149" s="28"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
@@ -4103,121 +4108,121 @@
       <c r="C150" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D150" s="24">
+      <c r="D150" s="25">
         <v>286056</v>
       </c>
-      <c r="G150" s="32"/>
+      <c r="G150" s="28"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C151" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="D151" s="24">
+      <c r="D151" s="25">
         <v>286057</v>
       </c>
-      <c r="G151" s="32"/>
+      <c r="G151" s="28"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
         <v>229</v>
       </c>
-      <c r="D152" s="23">
+      <c r="D152" s="22">
         <v>189565</v>
       </c>
-      <c r="G152" s="32"/>
+      <c r="G152" s="28"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
         <v>230</v>
       </c>
-      <c r="D153" s="23">
+      <c r="D153" s="22">
         <v>189914</v>
       </c>
-      <c r="G153" s="32"/>
+      <c r="G153" s="28"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C154" t="s">
         <v>231</v>
       </c>
-      <c r="D154" s="23">
+      <c r="D154" s="22">
         <v>190452</v>
       </c>
-      <c r="G154" s="32"/>
+      <c r="G154" s="28"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C155" t="s">
         <v>232</v>
       </c>
-      <c r="D155" s="23">
+      <c r="D155" s="22">
         <v>232155</v>
       </c>
-      <c r="G155" s="32"/>
+      <c r="G155" s="28"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
         <v>233</v>
       </c>
-      <c r="D156" s="23">
+      <c r="D156" s="22">
         <v>232268</v>
       </c>
-      <c r="G156" s="32"/>
+      <c r="G156" s="28"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C157" t="s">
         <v>234</v>
       </c>
-      <c r="D157" s="23">
+      <c r="D157" s="22">
         <v>232668</v>
       </c>
-      <c r="G157" s="32"/>
+      <c r="G157" s="28"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D158" s="24"/>
-      <c r="G158" s="32"/>
+      <c r="D158" s="25"/>
+      <c r="G158" s="28"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D159" s="24"/>
-      <c r="G159" s="32"/>
+      <c r="D159" s="25"/>
+      <c r="G159" s="28"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D160" s="24"/>
+      <c r="D160" s="25"/>
     </row>
     <row r="161" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D161" s="29"/>
+      <c r="D161" s="31"/>
     </row>
     <row r="162" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D162" s="29"/>
+      <c r="D162" s="31"/>
     </row>
     <row r="164" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D164" s="24"/>
+      <c r="D164" s="25"/>
     </row>
     <row r="165" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C165"/>
-      <c r="D165" s="24"/>
+      <c r="D165" s="25"/>
     </row>
     <row r="166" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C166"/>
-      <c r="D166" s="23"/>
+      <c r="D166" s="22"/>
     </row>
     <row r="167" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C167"/>
-      <c r="D167" s="23"/>
+      <c r="D167" s="22"/>
     </row>
     <row r="168" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C168"/>
-      <c r="D168" s="23"/>
+      <c r="D168" s="22"/>
     </row>
     <row r="169" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C169"/>
-      <c r="D169" s="23"/>
+      <c r="D169" s="22"/>
     </row>
     <row r="170" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C170"/>
-      <c r="D170" s="23"/>
+      <c r="D170" s="22"/>
     </row>
     <row r="171" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C171"/>
-      <c r="D171" s="23"/>
+      <c r="D171" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>